<commit_message>
Excel reporting & test improvements
</commit_message>
<xml_diff>
--- a/test/data/job10_eg.xlsx
+++ b/test/data/job10_eg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kfrb/Code/RoomJuggler/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61EB6F74-EB88-234E-8D38-2D2A8DB3148F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94CF92C1-17FA-0143-97DA-5402CDD0C7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="500" windowWidth="33520" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="500" windowWidth="33520" windowHeight="18840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="guests" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{A9C92AD2-9322-4845-A8E1-00D845A75F37}" name="guests10" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/kfrb/Code/RoomJuggler/test/data/guests10.csv" decimal="," thousands="." tab="0" semicolon="1">
+    <textPr sourceFile="/Users/kfrb/Code/RoomJuggler/test/data/guests10.csv" decimal="," thousands="." tab="0" semicolon="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -37,7 +37,7 @@
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{56B3162C-A4F4-434A-9C69-346851155D83}" name="rooms10" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/kfrb/Code/RoomJuggler/test/data/rooms10.csv" decimal="," thousands="." semicolon="1">
+    <textPr sourceFile="/Users/kfrb/Code/RoomJuggler/test/data/rooms10.csv" decimal="," thousands="." semicolon="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -46,7 +46,7 @@
     </textPr>
   </connection>
   <connection id="3" xr16:uid="{18D0F89F-C7C6-4343-9E73-44B1CFFC652F}" name="wishes10" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/kfrb/Code/RoomJuggler/test/data/wishes10.csv" decimal="," thousands="." semicolon="1">
+    <textPr sourceFile="/Users/kfrb/Code/RoomJuggler/test/data/wishes10.csv" decimal="," thousands="." semicolon="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>name</t>
   </si>
@@ -91,9 +91,6 @@
     <t>John Kinder</t>
   </si>
   <si>
-    <t>Cami Horton</t>
-  </si>
-  <si>
     <t>Asa Martell</t>
   </si>
   <si>
@@ -131,9 +128,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Mark White</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> John Kinder</t>
   </si>
   <si>
     <t>co123@web.com</t>
@@ -431,8 +425,8 @@
   </sheetPr>
   <dimension ref="A1:H301"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -471,16 +465,14 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
@@ -488,7 +480,7 @@
     </row>
     <row r="6" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>2</v>
@@ -496,7 +488,7 @@
     </row>
     <row r="7" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
@@ -504,7 +496,7 @@
     </row>
     <row r="8" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>2</v>
@@ -512,7 +504,7 @@
     </row>
     <row r="9" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>3</v>
@@ -520,7 +512,7 @@
     </row>
     <row r="10" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>3</v>
@@ -528,7 +520,7 @@
     </row>
     <row r="11" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>2</v>
@@ -1707,7 +1699,7 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView zoomScale="190" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1722,10 +1714,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1736,7 +1728,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1747,18 +1739,16 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2">
-        <v>2</v>
-      </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1769,7 +1759,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1969,8 +1959,8 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1988,14 +1978,12 @@
   <sheetData>
     <row r="1" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -2004,16 +1992,16 @@
     </row>
     <row r="2" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>

</xml_diff>